<commit_message>
Ergänzung um Funktionalität zur Behandlung von Klassenattributen.
git-svn-id: https://db-svn.informatik.uni-bremen.de/repos/stuff/use_plugins/ModelValidator/trunk@2422 e95982d2-0d12-e879-a455-8ce5a0885042
</commit_message>
<xml_diff>
--- a/src/org/tzi/use/modelvalidator/gui/MV_GUI_Anforderungen.xlsx
+++ b/src/org/tzi/use/modelvalidator/gui/MV_GUI_Anforderungen.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="24180" windowHeight="11220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ClassBounds" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Attributes" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:T36"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Class</t>
   </si>
@@ -52,6 +53,57 @@
   </si>
   <si>
     <t>Concrete (optional)</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ada-&gt;'Ada',bob-&gt;'Bob'</t>
+  </si>
+  <si>
+    <t>luckyNumbers</t>
+  </si>
+  <si>
+    <t>ada-&gt;Set{1,2,3}</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>Ada', 'Bob', 'Cyd', 'Dan'</t>
+  </si>
+  <si>
+    <t>numbers</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,12</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>1..100</t>
+  </si>
+  <si>
+    <t>ada-&gt;3</t>
+  </si>
+  <si>
+    <t>ages</t>
+  </si>
+  <si>
+    <t>Undefined fix</t>
+  </si>
+  <si>
+    <t>Set elements fix</t>
   </si>
 </sst>
 </file>
@@ -105,9 +157,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -405,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -437,7 +490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1">
+    <row r="2" spans="1:7" customFormat="1" ht="15.75" thickTop="1">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -451,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" customFormat="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -481,12 +534,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" customFormat="1" ht="15.75" thickTop="1"/>
+    <row r="3" spans="1:11" customFormat="1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>